<commit_message>
Added more data and more experiments
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Predictive-Text\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63704F40-DDDF-4E73-A236-C56EA4395813}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CE7F76-DBA2-4C78-8F45-7325829EAB97}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14880" yWindow="4065" windowWidth="14415" windowHeight="11535" xr2:uid="{91357438-6A8D-431F-ADAA-B2B9292682FB}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{91357438-6A8D-431F-ADAA-B2B9292682FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="53">
   <si>
     <t>Dataset</t>
   </si>
@@ -123,9 +123,6 @@
     <t>20200324-204855</t>
   </si>
   <si>
-    <t>Tweets, Github, FactBase</t>
-  </si>
-  <si>
     <t>GRU(Sequence Length, Unique Chars)</t>
   </si>
   <si>
@@ -157,13 +154,49 @@
   </si>
   <si>
     <t>20200324-225921</t>
+  </si>
+  <si>
+    <t>Training Time (Seconds)</t>
+  </si>
+  <si>
+    <t>Continued Training</t>
+  </si>
+  <si>
+    <t>20200325-014254</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>20200325-081236</t>
+  </si>
+  <si>
+    <t>Tweets, Github, FactBase(3/23)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One of the best models so far. Widening of the network incressed accuracy significantly. Also only using signle step. I think that this is fine and provides more training examples. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Continued training from the 20200324-204855 model. Training diverged. Accuracy fell significantly. Total epochs trained: 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Same model as 20200324-204855 but only trained on tweets. Using smaller dataset to try and get a model that can do better on training. </t>
+  </si>
+  <si>
+    <t>Slightly wider model than 20200324-220128.</t>
+  </si>
+  <si>
+    <t>Slightly deeper model than 20200324-220128.</t>
+  </si>
+  <si>
+    <t>SELU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,8 +226,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,6 +275,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -302,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -311,8 +364,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -342,9 +393,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -382,6 +430,59 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -676,434 +777,868 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F25FB23-8C6C-4F9B-9ED9-BA59A12A8B31}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.75" style="4" customWidth="1"/>
-    <col min="2" max="2" width="21" style="4" customWidth="1"/>
-    <col min="3" max="3" width="36.375" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="36.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="4"/>
+    <col min="1" max="1" width="24.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.375" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="36.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="41.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:9" s="11" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="38" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="36"/>
+      <c r="B2" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="31"/>
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="13">
+        <v>67</v>
+      </c>
+      <c r="D4" s="13">
+        <v>67</v>
+      </c>
+      <c r="E4" s="13">
+        <v>66</v>
+      </c>
+      <c r="F4" s="13">
+        <v>66</v>
+      </c>
+      <c r="G4" s="13">
+        <v>66</v>
+      </c>
+      <c r="H4" s="13">
+        <v>66</v>
+      </c>
+      <c r="I4" s="13"/>
+    </row>
+    <row r="5" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="31"/>
+      <c r="B5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="13">
+        <v>23321467</v>
+      </c>
+      <c r="D5" s="13">
+        <v>23321467</v>
+      </c>
+      <c r="E5" s="13">
+        <v>5204704</v>
+      </c>
+      <c r="F5" s="13">
+        <v>5204704</v>
+      </c>
+      <c r="G5" s="13">
+        <v>5204704</v>
+      </c>
+      <c r="H5" s="13">
+        <v>5204704</v>
+      </c>
+      <c r="I5" s="13"/>
+    </row>
+    <row r="6" spans="1:9" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="31"/>
+      <c r="B6" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="18">
+        <f>ROUNDDOWN(C5/C12-C11,0)</f>
+        <v>23321447</v>
+      </c>
+      <c r="D6" s="18">
+        <f>ROUNDDOWN(D5/D12-D11,0)</f>
+        <v>23321447</v>
+      </c>
+      <c r="E6" s="18">
+        <f>ROUNDDOWN(E5/E12-E11,0)</f>
+        <v>5204684</v>
+      </c>
+      <c r="F6" s="18">
+        <f>ROUNDDOWN(F5/F12-F11,0)</f>
+        <v>5204684</v>
+      </c>
+      <c r="G6" s="18">
+        <f>ROUNDDOWN(G5/G12-G11,0)</f>
+        <v>5204684</v>
+      </c>
+      <c r="H6" s="18">
+        <f>ROUNDDOWN(H5/H12-H11,0)</f>
+        <v>5204684</v>
+      </c>
+      <c r="I6" s="18"/>
+    </row>
+    <row r="7" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="31"/>
+      <c r="B7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="D7" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="E7" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="F7" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="G7" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="H7" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="I7" s="13"/>
+    </row>
+    <row r="8" spans="1:9" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="31"/>
+      <c r="B8" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="18">
+        <f>ROUNDDOWN(C6-C6*C7,0)</f>
+        <v>22155374</v>
+      </c>
+      <c r="D8" s="18">
+        <f>ROUNDDOWN(D6-D6*D7,0)</f>
+        <v>22155374</v>
+      </c>
+      <c r="E8" s="18">
+        <f>ROUNDDOWN(E6-E6*E7,0)</f>
+        <v>4944449</v>
+      </c>
+      <c r="F8" s="18">
+        <f>ROUNDDOWN(F6-F6*F7,0)</f>
+        <v>4944449</v>
+      </c>
+      <c r="G8" s="18">
+        <f>ROUNDDOWN(G6-G6*G7,0)</f>
+        <v>4944449</v>
+      </c>
+      <c r="H8" s="18">
+        <f>ROUNDDOWN(H6-H6*H7,0)</f>
+        <v>4944449</v>
+      </c>
+      <c r="I8" s="18"/>
+    </row>
+    <row r="9" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="32"/>
+      <c r="B9" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="18">
+        <f>ROUNDUP(C6*C7,0)</f>
+        <v>1166073</v>
+      </c>
+      <c r="D9" s="18">
+        <f>ROUNDUP(D6*D7,0)</f>
+        <v>1166073</v>
+      </c>
+      <c r="E9" s="18">
+        <f>ROUNDUP(E6*E7,0)</f>
+        <v>260235</v>
+      </c>
+      <c r="F9" s="18">
+        <f>ROUNDUP(F6*F7,0)</f>
+        <v>260235</v>
+      </c>
+      <c r="G9" s="18">
+        <f>ROUNDUP(G6*G7,0)</f>
+        <v>260235</v>
+      </c>
+      <c r="H9" s="18">
+        <f>ROUNDUP(H6*H7,0)</f>
+        <v>260235</v>
+      </c>
+      <c r="I9" s="18"/>
+    </row>
+    <row r="10" spans="1:9" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="D10" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="E10" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="F10" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="G10" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="H10" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="I10" s="14"/>
+    </row>
+    <row r="11" spans="1:9" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="25"/>
+      <c r="B11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="14">
+        <v>20</v>
+      </c>
+      <c r="D11" s="14">
+        <v>20</v>
+      </c>
+      <c r="E11" s="14">
+        <v>20</v>
+      </c>
+      <c r="F11" s="14">
+        <v>20</v>
+      </c>
+      <c r="G11" s="14">
+        <v>20</v>
+      </c>
+      <c r="H11" s="14">
+        <v>20</v>
+      </c>
+      <c r="I11" s="14"/>
+    </row>
+    <row r="12" spans="1:9" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25"/>
+      <c r="B12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="14">
+        <v>1</v>
+      </c>
+      <c r="D12" s="14">
+        <v>1</v>
+      </c>
+      <c r="E12" s="14">
+        <v>1</v>
+      </c>
+      <c r="F12" s="14">
+        <v>1</v>
+      </c>
+      <c r="G12" s="14">
+        <v>1</v>
+      </c>
+      <c r="H12" s="14">
+        <v>1</v>
+      </c>
+      <c r="I12" s="14"/>
+    </row>
+    <row r="13" spans="1:9" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="25"/>
+      <c r="B13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="14">
+        <v>124</v>
+      </c>
+      <c r="D13" s="14">
+        <v>124</v>
+      </c>
+      <c r="E13" s="14">
+        <v>124</v>
+      </c>
+      <c r="F13" s="14">
+        <v>124</v>
+      </c>
+      <c r="G13" s="14">
+        <v>124</v>
+      </c>
+      <c r="H13" s="14">
+        <v>124</v>
+      </c>
+      <c r="I13" s="14"/>
+    </row>
+    <row r="14" spans="1:9" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="26"/>
+      <c r="B14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="14">
+        <v>2</v>
+      </c>
+      <c r="D14" s="14">
+        <v>8</v>
+      </c>
+      <c r="E14" s="14">
+        <v>6</v>
+      </c>
+      <c r="F14" s="14">
+        <v>6</v>
+      </c>
+      <c r="G14" s="14">
+        <v>6</v>
+      </c>
+      <c r="H14" s="14">
+        <v>6</v>
+      </c>
+      <c r="I14" s="14"/>
+    </row>
+    <row r="15" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="8">
+        <v>2</v>
+      </c>
+      <c r="D15" s="8">
+        <v>2</v>
+      </c>
+      <c r="E15" s="15">
+        <v>4</v>
+      </c>
+      <c r="F15" s="15">
+        <v>5</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+    </row>
+    <row r="16" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="22"/>
+      <c r="B16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="15">
+        <v>0.65</v>
+      </c>
+      <c r="D16" s="15">
+        <v>0.65169999999999995</v>
+      </c>
+      <c r="E16" s="15">
+        <v>0.62909999999999999</v>
+      </c>
+      <c r="F16" s="15">
+        <v>0.62890000000000001</v>
+      </c>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+    </row>
+    <row r="17" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="22"/>
+      <c r="B17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="15">
+        <v>1.1698</v>
+      </c>
+      <c r="D17" s="15">
+        <v>1.1628000000000001</v>
+      </c>
+      <c r="E17" s="8">
+        <v>1.2732000000000001</v>
+      </c>
+      <c r="F17" s="8">
+        <v>1.2736000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="23"/>
+      <c r="B18" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="34"/>
+      <c r="D18" s="40">
+        <v>2700</v>
+      </c>
+      <c r="E18" s="8">
+        <v>630</v>
+      </c>
+      <c r="F18" s="8">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="15">
+        <v>0.66190000000000004</v>
+      </c>
+      <c r="D19" s="15">
+        <v>0.66178000000000003</v>
+      </c>
+      <c r="E19" s="15">
+        <v>0.59347000000000005</v>
+      </c>
+      <c r="F19" s="15">
+        <v>0.59216999999999997</v>
+      </c>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+    </row>
+    <row r="20" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="23"/>
+      <c r="B20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="15">
+        <v>1.1111</v>
+      </c>
+      <c r="D20" s="15">
+        <v>1.1027</v>
+      </c>
+      <c r="E20" s="15">
+        <v>1.4321999999999999</v>
+      </c>
+      <c r="F20" s="15">
+        <v>1.4197</v>
+      </c>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+    </row>
+    <row r="21" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="I21" s="16"/>
+    </row>
+    <row r="22" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="28"/>
+      <c r="B22" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="I22" s="17"/>
+    </row>
+    <row r="23" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="28"/>
+      <c r="B23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34"/>
-      <c r="B3" s="5" t="s">
+      <c r="G23" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23" s="17"/>
+    </row>
+    <row r="24" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="28"/>
+      <c r="B24" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H24" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="I24" s="17"/>
+    </row>
+    <row r="25" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="28"/>
+      <c r="B25" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="15">
-        <v>67</v>
-      </c>
-      <c r="D3" s="15">
-        <v>66</v>
-      </c>
-      <c r="E3" s="15">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="34"/>
-      <c r="B4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="15">
-        <v>23321467</v>
-      </c>
-      <c r="D4" s="15">
-        <v>5204704</v>
-      </c>
-      <c r="E4" s="15">
-        <v>5204704</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="34"/>
-      <c r="B5" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="20">
-        <f>ROUNDDOWN(C4/C11-C10,0)</f>
-        <v>23321447</v>
-      </c>
-      <c r="D5" s="20">
-        <f>ROUNDDOWN(D4/D11-D10,0)</f>
-        <v>5204684</v>
-      </c>
-      <c r="E5" s="20">
-        <f>ROUNDDOWN(E4/E11-E10,0)</f>
-        <v>5204684</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="34"/>
-      <c r="B6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="15">
-        <v>0.05</v>
-      </c>
-      <c r="D6" s="15">
-        <v>0.05</v>
-      </c>
-      <c r="E6" s="15">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="34"/>
-      <c r="B7" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="20">
-        <f>ROUNDDOWN(C5-C5*C6,0)</f>
-        <v>22155374</v>
-      </c>
-      <c r="D7" s="20">
-        <f>ROUNDDOWN(D5-D5*D6,0)</f>
-        <v>4944449</v>
-      </c>
-      <c r="E7" s="20">
-        <f>ROUNDDOWN(E5-E5*E6,0)</f>
-        <v>4944449</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="35"/>
-      <c r="B8" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="20">
-        <f>ROUNDUP(C5*C6,0)</f>
-        <v>1166073</v>
-      </c>
-      <c r="D8" s="20">
-        <f>ROUNDUP(D5*D6,0)</f>
-        <v>260235</v>
-      </c>
-      <c r="E8" s="20">
-        <f>ROUNDUP(E5*E6,0)</f>
-        <v>260235</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="16">
-        <v>1E-3</v>
-      </c>
-      <c r="D9" s="16">
-        <v>1E-3</v>
-      </c>
-      <c r="E9" s="16">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="28"/>
-      <c r="B10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="16">
-        <v>20</v>
-      </c>
-      <c r="D10" s="16">
-        <v>20</v>
-      </c>
-      <c r="E10" s="16">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="28"/>
-      <c r="B11" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="16">
-        <v>1</v>
-      </c>
-      <c r="D11" s="16">
-        <v>1</v>
-      </c>
-      <c r="E11" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="28"/>
-      <c r="B12" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="16">
-        <v>124</v>
-      </c>
-      <c r="D12" s="16">
-        <v>124</v>
-      </c>
-      <c r="E12" s="16">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="29"/>
-      <c r="B13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="16">
-        <v>2</v>
-      </c>
-      <c r="D13" s="16">
-        <v>6</v>
-      </c>
-      <c r="E13" s="16">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="10">
-        <v>2</v>
-      </c>
-      <c r="D14" s="17">
+      <c r="D25" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="17"/>
-    </row>
-    <row r="15" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="25"/>
-      <c r="B15" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="17">
-        <v>0.65</v>
-      </c>
-      <c r="D15" s="17">
-        <v>0.62909999999999999</v>
-      </c>
-      <c r="E15" s="17"/>
-    </row>
-    <row r="16" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="26"/>
-      <c r="B16" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="17">
-        <v>1.1698</v>
-      </c>
-      <c r="D16" s="10">
-        <v>1.2732000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="17">
-        <v>0.66190000000000004</v>
-      </c>
-      <c r="D17" s="17">
-        <v>0.59347000000000005</v>
-      </c>
-      <c r="E17" s="17"/>
-    </row>
-    <row r="18" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="26"/>
-      <c r="B18" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="17">
-        <v>1.1111</v>
-      </c>
-      <c r="D18" s="17">
-        <v>1.4321999999999999</v>
-      </c>
-      <c r="E18" s="17"/>
-    </row>
-    <row r="19" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="31"/>
-      <c r="B20" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="19" t="s">
+      <c r="E25" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="H25" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="I25" s="17"/>
+    </row>
+    <row r="26" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="28"/>
+      <c r="B26" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="I26" s="17"/>
+    </row>
+    <row r="27" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="28"/>
+      <c r="B27" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="G27" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="H27" s="17" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="31"/>
-      <c r="B21" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="19" t="s">
+      <c r="I27" s="17"/>
+    </row>
+    <row r="28" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="28"/>
+      <c r="B28" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="H28" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="I28" s="17"/>
+    </row>
+    <row r="29" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="28"/>
+      <c r="B29" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="H29" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="I29" s="16"/>
+    </row>
+    <row r="30" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="29"/>
+      <c r="B30" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="H30" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="31"/>
-      <c r="B22" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="31"/>
-      <c r="B23" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="31"/>
-      <c r="B24" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="31"/>
-      <c r="B25" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-    </row>
-    <row r="26" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="31"/>
-      <c r="B26" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-    </row>
-    <row r="27" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="31"/>
-      <c r="B27" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-    </row>
-    <row r="28" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="32"/>
-      <c r="B28" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+    </row>
+    <row r="31" spans="1:9" s="44" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="42"/>
+      <c r="C31" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="E31" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="F31" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="G31" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="H31" s="43"/>
+      <c r="I31" s="43"/>
+    </row>
+    <row r="32" spans="1:9" s="44" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="45"/>
+      <c r="B32" s="46"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="47"/>
+    </row>
+    <row r="33" spans="1:9" s="44" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="45"/>
+      <c r="B33" s="46"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="47"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="47"/>
+    </row>
+    <row r="34" spans="1:9" s="44" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="45"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="47"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="47"/>
+      <c r="H34" s="47"/>
+      <c r="I34" s="47"/>
+    </row>
+    <row r="35" spans="1:9" s="44" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="48"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="50"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C36" s="4"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C37" s="4"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C38" s="4"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C39" s="4"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C40" s="4"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C41" s="4"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C42" s="4"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C43" s="4"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C44" s="4"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C45" s="4"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C46" s="4"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C47" s="4"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C48" s="4"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C49" s="4"/>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C50" s="4"/>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C51" s="4"/>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C52" s="4"/>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C53" s="4"/>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C54" s="4"/>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C55" s="4"/>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C56" s="4"/>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C57" s="4"/>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C58" s="4"/>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C59" s="4"/>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C60" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A9:A13"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A28"/>
-    <mergeCell ref="A2:A8"/>
+  <mergeCells count="15">
+    <mergeCell ref="G31:G35"/>
+    <mergeCell ref="I31:I35"/>
+    <mergeCell ref="H31:H35"/>
+    <mergeCell ref="B31:B35"/>
+    <mergeCell ref="E31:E35"/>
+    <mergeCell ref="D31:D35"/>
+    <mergeCell ref="C31:C35"/>
+    <mergeCell ref="F31:F35"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A30"/>
+    <mergeCell ref="A3:A9"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A31:A35"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="A17:D17 F17:XFD17">
-    <cfRule type="dataBar" priority="8">
+  <conditionalFormatting sqref="D19">
+    <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1111,13 +1646,13 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{154CA1A9-5B92-49D0-9781-4BC82293A437}</x14:id>
+          <x14:id>{E6E3E41A-14D0-4720-8B5E-8641BC28E69C}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E17">
-    <cfRule type="dataBar" priority="4">
+  <conditionalFormatting sqref="A19:C19 J19:XFD19 E19:G19">
+    <cfRule type="dataBar" priority="21">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1125,13 +1660,27 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2E1AD879-2F9D-499C-A271-6A840CE1E46E}</x14:id>
+          <x14:id>{7CA4FA6C-7045-4F0E-9654-94515F47C232}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4:XFD4">
-    <cfRule type="dataBar" priority="2">
+  <conditionalFormatting sqref="I19">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFD6007B"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{A4EE9D10-C17D-4B80-8B1A-08BBE3A235AA}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5:G6 I5:XFD6">
+    <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1139,12 +1688,26 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3CDA93A5-C424-4140-8091-ECA3780DB59E}</x14:id>
+          <x14:id>{6B68132B-A6F7-4F6F-A0F8-29354752C3BE}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:XFD5">
+  <conditionalFormatting sqref="H19">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFD6007B"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{714955FD-0BC1-4354-A4E4-501566E80D0B}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:H6">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -1153,7 +1716,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{CBE5176C-0F23-4613-90AC-7AFCBC6A80F4}</x14:id>
+          <x14:id>{3753BF0B-DD80-425B-8A2F-FA85D4A94618}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -1164,7 +1727,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{154CA1A9-5B92-49D0-9781-4BC82293A437}">
+          <x14:cfRule type="dataBar" id="{E6E3E41A-14D0-4720-8B5E-8641BC28E69C}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -1174,10 +1737,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>A17:D17 F17:XFD17</xm:sqref>
+          <xm:sqref>D19</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2E1AD879-2F9D-499C-A271-6A840CE1E46E}">
+          <x14:cfRule type="dataBar" id="{7CA4FA6C-7045-4F0E-9654-94515F47C232}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -1187,10 +1750,23 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E17</xm:sqref>
+          <xm:sqref>A19:C19 J19:XFD19 E19:G19</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3CDA93A5-C424-4140-8091-ECA3780DB59E}">
+          <x14:cfRule type="dataBar" id="{A4EE9D10-C17D-4B80-8B1A-08BBE3A235AA}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFD6007B"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I19</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{6B68132B-A6F7-4F6F-A0F8-29354752C3BE}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -1200,10 +1776,23 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>A4:XFD4</xm:sqref>
+          <xm:sqref>A5:G6 I5:XFD6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{CBE5176C-0F23-4613-90AC-7AFCBC6A80F4}">
+          <x14:cfRule type="dataBar" id="{714955FD-0BC1-4354-A4E4-501566E80D0B}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFD6007B"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H19</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{3753BF0B-DD80-425B-8A2F-FA85D4A94618}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -1213,7 +1802,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>A5:XFD5</xm:sqref>
+          <xm:sqref>H5:H6</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>